<commit_message>
paper -- adding GWAS results
</commit_message>
<xml_diff>
--- a/paper/DiscussionBrainstorm.xlsx
+++ b/paper/DiscussionBrainstorm.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>observation</t>
   </si>
@@ -25,6 +25,36 @@
   </si>
   <si>
     <t>extension</t>
+  </si>
+  <si>
+    <t>domesticated hosts show more variable lesion size</t>
+  </si>
+  <si>
+    <t>overlap between wild and domesticated host lesion size</t>
+  </si>
+  <si>
+    <t>isolate order changes depending on host</t>
+  </si>
+  <si>
+    <t>bo5.10 is an average isolate</t>
+  </si>
+  <si>
+    <t>many genes are found w large lesion effects</t>
+  </si>
+  <si>
+    <t>effect size of largest genes depends on plant host</t>
+  </si>
+  <si>
+    <t>strongly multigenic trait</t>
+  </si>
+  <si>
+    <t>domestication has a host-dependent effect on resistance</t>
+  </si>
+  <si>
+    <t>domestication did not reduce genetic diversity for lesion size</t>
+  </si>
+  <si>
+    <t>DmWoD hits nonoverlapping with D or W</t>
   </si>
 </sst>
 </file>
@@ -363,16 +393,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.140625" customWidth="1"/>
-    <col min="2" max="2" width="44.5703125" customWidth="1"/>
+    <col min="1" max="1" width="52.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -385,6 +415,50 @@
       </c>
       <c r="C1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>